<commit_message>
Get daily reddit data: Tue Aug  5 08:14:28 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_10.xlsx
+++ b/data/collected_data/2025_08_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C519"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3712 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1mi2p0g</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Ocean vibes 🦈🌊🪼🐚</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8z7sq8pal5hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1mi20c5</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Moon child 🌚</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19tmhrmjd5hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1mi1bgn</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>No flash</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cha8qt4x55hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1mi1bht</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Sharks and waves</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16yoh4ex55hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1mi1atx</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8mreaeq55hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1mi1aev</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>🧈</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eew1qgcm55hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1mi12y9</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>CO Nail tech recs!!</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mi12y9/co_nail_tech_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1mi0xzr</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>my ice cream themed birthday nails 🩷🍦</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvznwgvv15hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1mi0w34</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>A lil shimmer, a lil shine💅💕</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9kpaqbx05hf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1mi0izp</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>mermaidy nails i did today!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi0izp</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1mhzo1g</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Good colors</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a05ns2vzo4hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1mhzifj</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Manicure look, at home application</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhzifj</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1mhzglu</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Curing press-on nails not always necessary?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mhzglu/curing_presson_nails_not_always_necessary/</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1mhxhgp</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Short nail bed problems?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mhxhgp/short_nail_bed_problems/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1mhx33l</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Do you like it? I made it for a wedding party :)</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kwyeaoy14hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1mhwvzq</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>some strawberry shortcake nails i did !</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhwvzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1mhwq3j</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Festival Nails lo</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhwq3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1mhw2lx</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Soft pink mermaid nails</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhw2lx</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1mhv8x2</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Why do my thumbs always look like ramps from the side? Is it my natural nail bed doing this?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwrpcx23n3hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1mhvr11</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Summer nail dump 💅🏼☀️🍒</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhvr11</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1mhv8s3</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>I think it’s safe to say these are the best nails I’ve ever done 😇 (Swipe for my clean gel-x application 😍)</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhv8s3</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1mhuorb</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Help finding this shade</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oa2kuptji3hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1mhtz24</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Beginner here but I tried to make a kpop demon hunters set!</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mixiwk6tc3hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1mhtjvl</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Birthday nails!!</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujgouwcg93hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1mhtjgg</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Generous tips- reduce amount?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mhtjgg/generous_tips_reduce_amount/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1mhtd9b</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Opi - I’m Yacht Leaving</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50bkeiv083hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1mhszu7</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>my favorites 🥰</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhszu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1mhszsf</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Can’t keep my cuticles moisturized</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mhszsf/cant_keep_my_cuticles_moisturized/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1mhsxp5</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>I’m obsessed 😭</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhsxp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1mhsoig</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>🍒🍒</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhsoig</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1mhsm9c</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>💖sparkle sparkle</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/agzhp4xb23hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1mhse4j</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Best brand of press on nails</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mhse4j/best_brand_of_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1mhsblp</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Who else thinks polka dots nails are literally the cutest?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5tmtef303hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1mhsav1</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>So happy with my nails! ✨☁️</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j21hv5sxz2hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1mhsa73</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Is "holo picnic blueberry" a good description? 🫐✨️</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4urigusz2hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1mhs9r9</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Went to a new nail tech</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhs9r9</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1mhs2pd</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time in forever</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhs2pd</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1mhs182</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>What polish would give this effect?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mhs182/what_polish_would_give_this_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1mhq4az</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Help with a product?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhq4az</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1mhqqxn</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>New to getting my nails done and not sure etiquette</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mhqqxn/new_to_getting_my_nails_done_and_not_sure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1mhrair</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Are my acrylic nails too thick?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhrair</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1mhqoeb</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Gyaru nails</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4iu26ctao2hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1mhqit9</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>What do you think of this design? My brother made them</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4eq6q454n2hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1mhqis9</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>My version of fish nails I’ve seen all over online!</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhqis9</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1mhpbru</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Chrome Zebra Stripes and Spicy Red🔥🦓🔥</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhpbru</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1mhp98w</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Some shorties!</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhp98w</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1mhp7kq</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>beautiful❤️</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q65v3ggde2hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1mhowtv</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Finished painting my hunchback of notre dame nail set for my display 🤭</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9f9n36sdc2hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1mho270</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Unbelievable nails</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3100ywlo62hf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1mho0it</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Practicing Acrylic</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mho0it</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1mhncjb</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>The pain the burn - UV gel</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21r1nk3y12hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1mhn6zs</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Shifty Business 🌌</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhn6zs</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1mhmr9y</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Best home polish for thin nails that peel easily?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mhmr9y/best_home_polish_for_thin_nails_that_peel_easily/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1mhmicy</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Cat Eye</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhmicy</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1mhmd3f</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time, hoping it turned out well!!</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adpql0giv1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1mhlj22</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>How do you rate my new work? 🐚</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4ct96y2q1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1mhl9aw</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>What is this color considered?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sfbgywbo1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1mhlpo3</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Dark Fairy Nails</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oez8zam9r1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1mhjtov</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Opinion needed - which shape? Part 2!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhjtov</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1mhkc3k</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>My daughter is 10 and she did her own “Magic 8-Ball” nails</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhkc3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1mhk5kw</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>I’m working on a Salvador Dali set!</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3r91xzieh1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1mhj02d</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>How to Make Short Almond Nails Look Good</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhj02d</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1mh6971</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>How do I avoid this when I do press ons?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mh6971</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1mh6dyk</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Long nail friendly gloves</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mh6dyk/long_nail_friendly_gloves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1mh8k9t</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>All my nails are curling inwards</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mh8k9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1mhdlds</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Glue-On Disaster</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhdlds</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1mhfy4z</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Need advice…</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhfy4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1mhi6e6</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>First time getting builder gel</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhi6e6</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1mhft3r</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Give it to me straight!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhft3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1mhhqiw</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>My Nails Look Like Rubies</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2dkrlmo11hf1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1mhh9t3</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>What shape and length is best?</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhh9t3</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1mhh8lf</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Got these done and omg my tech did such an amazing job!</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spn5fdyfy0hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1mhh2kp</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Biab has been the holy grail</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1yp5rzqbx0hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1mhfr5k</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Thoughts on Kiss Powerflex?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mhfr5k/thoughts_on_kiss_powerflex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1mhfmjw</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>French with a soft pink base</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1ky159sn0hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1mheivk</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Should I cut them ?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31899es3g0hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1mhed09</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Nails keep breaking in the same spot</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24xwbtcze0hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1mheabn</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mheabn</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1mhdutl</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Very simple but I love it</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhdutl</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1mhdexz</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Finally got my nail shape and length exactly right</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iv0cviq980hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1mhdcf2</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Pink chrome! 🎀</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzjdj33r70hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1mhdbaj</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Please help me make my nails better</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhbielri70hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1mhd53p</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>First attempt on French nails</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3uqrhfv660hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1mhd18y</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I did Gelish on my natural nails</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhd18y</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1mhcwts</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>simple fresh nails 🥰</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib6zqebg40hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1mhcald</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Please influence meeee💅</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mhcald/please_influence_meeee/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1mhbyye</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Some people were douchebags in the other guy's nail thread so I'm posting mine too.</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxog55zmwzgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1mhbcnd</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Btartbox Nails</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6d6zwnrprzgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1mhb8ln</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>My fav nails of the year! 💅🏾✨</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhb8ln</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1mhb52d</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>My boyfriend says they look like Rainbow candy nails</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhb52d</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1mhb2x4</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Painted my natural nails. Idk what else I can do to make them pop</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8qwh4p9pzgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1mhb0f5</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Soft nails that create 😍 auras, 3D flower relief, a true beauty ✔️</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exnofa4mozgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1mhac4i</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Got engaged so scared to show my man my feet- insecure help</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nf4g7hbizgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1mhaadd</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>My first DIY 3D Holiday nails. Can I be proud?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5ifl32whzgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1mha0yr</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Recent nail designs 🥰</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mha0yr</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1mh9i4o</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>They know what they’re doing in Romania, y’all.</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxu9ehxj9zgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1mh9ds8</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Black matte and kitties 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74cynax78zgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1mh8ysp</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Going to France and wanted something museum-esque, Mercury did not disappoint 🖼️</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mh8ysp</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1mh82qt</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>First time getting nails done</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mh82qt</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1mh7s3u</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Like my nails?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4v377q1qpygf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1mi1mnv</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Help! Can’t find this brand anywhere</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi1mnv</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1mi1jtn</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Matte top coat recommendations</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mi1jtn/matte_top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1mi1eqv</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Please help me choose a nail shape, I don’t know what I’m doing!</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi1eqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1mi07gp</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>My nails may smell like garlic, but they look like *gemstones*</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi07gp</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1mhypij</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>california love ✨</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhypij</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1mhxt96</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Split between the two because I couldn’t choose!</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i14ijrv484hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1mhxri7</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Chrome magic!</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6jzx67wv74hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1mhxn0i</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>All time favorite magnetic</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhxn0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1mhxj26</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>a different kind of fun with magnets</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9irtdz0t54hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1mhx571</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Where do yall get your stamping plates?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mhx571/where_do_yall_get_your_stamping_plates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1mhx4t8</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Nail polish reqs- allergic to HEMA</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mhx4t8/nail_polish_reqs_allergic_to_hema/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1mhww09</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Monarch Lacquer - Formula</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pmd4qn6oz3hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1mhw6og</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Ride the lightning 🌩</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhw6og</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1mhvzhs</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Worth the Wait 😍</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhvzhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1mhv6dr</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Dupe for Orly Kiss Me, I’m Kind?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mhv6dr/dupe_for_orly_kiss_me_im_kind/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1mhv1px</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>hello fellow canadians</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhv1px</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1mhuow2</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Which glass files are faster than 180-course?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mhuow2/which_glass_files_are_faster_than_180course/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1mhugi8</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>i have no one to show this to !!!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhugi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1mhu8en</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Solars &amp; Sunscreen - a test!</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhu8en</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1mhu55i</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Been wanting to try a Revlon</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhu55i</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1mhtput</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>July manicures in order ish</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhtput</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1mhtivd</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Bootleg Rotten Bananas</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhtivd</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1mhtfoj</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Magnetic Magic 🧲</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1exsofj83hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1mht5sw</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Couldn’t choose just one color…</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzxx3e1h63hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1mht07j</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>holo there 👋👋</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mht07j</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1mhsgkm</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Do you have mani pictures of any red polishes by Cracked?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mhsgkm/do_you_have_mani_pictures_of_any_red_polishes_by/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1mhs0of</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>First ILNP order, are there Coupon codes? Are these choices good?</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dt6m52fvx2hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1mhrzdo</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Was sad after salon visit so I did them myself 6 days later</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qqw4bvjlx2hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1mhrl5w</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Does lights lacquer have a Facebook group?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mhrl5w/does_lights_lacquer_have_a_facebook_group/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1mhqzg6</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>What is your go to AFFORDABLE nail polish brand</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mhqzg6/what_is_your_go_to_affordable_nail_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1mhq1ia</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Okay Atomic Polish 🤩🩷🧡</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhq1ia</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1mhpuwk</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>All the bubble wrap</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhpuwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1mhpj6c</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Among the sassiest of sauces…</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uhze6n7jg2hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1mhpbu9</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>ILNP mega</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhpbb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1mhp353</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Another Glass Cabochon Post</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3ud91sjd2hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1mhozbn</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>File?</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmxkwjyqb2hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1mhorq0</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Bee's Knees really did that</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhorq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1mho345</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Wish come true</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mho345</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1mhnzsd</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>nails for working in retail? (don't say short nails, i'm looking for medium to long)</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mhnzsd/nails_for_working_in_retail_dont_say_short_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1mhnw9i</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>💚 Cuticula Dead House 💜</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhnw9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1mhnkzv</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Bees Knees Lacquer IEANE</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhnkzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1mhnev0</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Looking for a polish the shade of vintage green glassware (pictured)… any recs?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/F8uKUVD.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1mhn8w2</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Shifty Business 🌌</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhn8w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1mhn1gp</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Favorite highlighter/neon yellow polish?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mhn1gp/favorite_highlighterneon_yellow_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1mhmz4y</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>My polish is pt approved lol</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkr83soez1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1mhmrol</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Science is Pretty - Tyler’s Trinkets (PPU Rewind ‘25)</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uc08yi44y1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1mhmr00</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Told the Northern Lights to Keep Shining</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/66hl7cfzx1hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1mhlt9y</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>“If you love me you will build something for me” worked!!</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ykiwv18xr1hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1mhlrbt</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Ford Cyber Orange Polish</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzhvcngkr1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1mhllkv</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Here’s a random collection of my past nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhllkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1mhllkl</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Was inspired by a few posts on here to swatch my whole collection in a swatch book!!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhllkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1mhlgdc</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>My most whimsical nails yet</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhlgdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1mhl5w7</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Who Do I Contact?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhl5w7</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1mhkwon</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>So Fiery Like Rengoku (iykyk)</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhkwon</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1mhkknq</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>how do I fix my nail bed shape?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nzstqxk2k1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1mhkdel</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>7000 Nail Geeks</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ih227iysi1hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1mhk9ol</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Finally gave up on forcing them to be almond shaped</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhk9ol</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1mhk6a5</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>orange and green !!</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhk6a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1mhk3jv</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Help me ID these OPI minis?</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhk3jv</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1mhk17k</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Salon mani w Dazzle Dry</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhk17k</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1mhjtvt</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Magnetics Make the DMV Bearable</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vbnitdc7f1hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1mhjqa9</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Pastel Neon Tangerine</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1434vaqoe1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1mhjofb</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Are we still only wearing nudes and neutrals to interviews and office jobs?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mhjofb/are_we_still_only_wearing_nudes_and_neutrals_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1mhjnqn</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>I ALSO did the glass bead on Psilocybin and holy rainbow 😮</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/oBoMqBylCjo?si=CqYm9WltXfp07WWj</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1mhjgfa</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>First time using a flakie topper, it’s like a new door has just opened to me!</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7ssp6jxc1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1mhj6up</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Mystery box fail</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhj6up</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1mhiz0n</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Polish with a deep aqua blue base with green highlight/color shift and no glitter?</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcy1wqbl91hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1mhig8p</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Finally received my ppu from last month!!</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhig8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1mhif1a</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>404: Soul Not Found is that girl</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86ebgiy061hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1mhid73</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>My first color changing pigmentsn</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwd9lo4u51hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1mhibqr</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Any advice on anything ?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uk5e9nnk51hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1mhi3a7</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Love this color!</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1pnq68141hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1mhhz7q</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Scarab Queen Dreams is what I'm calling these beauties</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlvpcsb931hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1mgtxdr</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Best Gel Magnetic Polish for velvet/cat eye nails</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mgtxdr/best_gel_magnetic_polish_for_velvetcat_eye_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1mhh8fe</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Birthday Rewards?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mhh8fe/birthday_rewards/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1mhh7x6</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Anyone know of a regular polish dupe for a color like this? Or a combo to get roughly the same look 🤔</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0u9p6boby0hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1mhgj7v</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Mobius by Cirque Colors</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmux98art0hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1mhesxk</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>I love every shade of green!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8yobxe1i0hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1mhegbm</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Love the "your nails but better" look! (Active Glow)</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhegbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1mhe9uo</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Best way to fix a nail break at home?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hddwtmide0hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1mhe9ll</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>I don’t care if it’s not popular, I LOVE ORANGE!!!</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhe9ll</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1mhccdo</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>The way this polish changes colors is incredible! ✨</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhccdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1mhb8j9</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>So Peachy!</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8uc4plooqzgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1mh9c5k</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mh9c5k/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1mh8err</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Finally got my nails to a nice length</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mh8err</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1mi236f</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Rate my nail art as a beginner</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ao69woihe5hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1mhiojz</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Practiced nails on myself</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7th5l1vx71hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1mi0prd</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>My bf wanted to show off his nails</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi0prd</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1mhzgre</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Sandy toes, starfish nails, and salty kisses 🌊⭐️💅</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e5ytkwl1n4hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1mhyos0</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Dew Drop Nature Inspired Set</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhyos0</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1mhxvu8</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Birthday nail set for my friend</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qcg5ufx84hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1mhwflt</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Does anyone have picture of a black to white gradient design?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbmm3mfvw3hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1mhvvmn</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>A few of my favorite press on sets from recently</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhvvmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1mhv2s6</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Please help me pick which one to wear to Disney!</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mhv2s6/please_help_me_pick_which_one_to_wear_to_disney/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1mhuq3y</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>💚</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7aa53xcti3hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1mhthqi</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Any Perfect Match fans?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjwikhdz83hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1mhth17</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Some fun clouds (first time painting my nails in years so don’t mind the messiness 😂)</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e79u36ut83hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1mhsfw4</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>First try!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhsfw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1mhs684</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Tortoiseshell!</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwnje8kzy2hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1mhry11</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>need help</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhry11</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1mhow60</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Finished painting my hunchback of notre dame nail set for my display 🤭</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkwiq9r9c2hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1mhot0a</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Advice needed</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mhot0a/advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1mhmjuk</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Nails for the parade!</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhmjuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1mhmd3r</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>The real one don't move while I'm doing nailart..</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjbhhqpiv1hf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1mhmac0</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Did two sets of press ons today 💕</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhmac0</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1mhkzoa</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Summer Psychedelic</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhkzoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1mhks8a</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Mylee Builder Gel with French tip, but the French tip is peeling - any idea why?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mhks8a/mylee_builder_gel_with_french_tip_but_the_french/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1mhkkd3</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Beach Nails</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3qj9nl0k1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1mhje7x</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>bubbles and starfishes</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ygqq4fjc1hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1mhipr0</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>My 5th nailart set</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhipr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1mhi3zd</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>my favourite holographic cateye.</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhi3zd</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1mhg71v</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkfgqskjr0hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1mhbaze</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>I love my nails! 🖤</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhbaze</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1mham6o</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Nailss💅</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mham6o/nailss/</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1mhaeve</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>SummerWeen 25 👻☀️</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mhaeve</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1mh93tc</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>3d flowers 🌺</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mh93tc</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1mh80pv</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Moon child ✨️</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2xjzgmlsygf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1mgypqb</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>How were they?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6pomcac9wgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Aug  6 08:14:32 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_10.xlsx
+++ b/data/collected_data/2025_08_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C519"/>
+  <dimension ref="A1:C707"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9256,6 +9256,3202 @@
         </is>
       </c>
     </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1miy9r1</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Help me have pretty nails!</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1miy9r1/help_me_have_pretty_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1mixwfk</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Best regular nail polishes</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mixwfk/best_regular_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1mixtpg</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>💙🤍</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fog0o0htlchf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1mivzmw</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Would dip powder work better for me?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mivzmw/would_dip_powder_work_better_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1mioy45</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>A tale of poor nail bed care at salons</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfbx3anxcahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1mimg51</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Nail ideas?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mimg51</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1mima89</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Looking for NYC nail recommendations!!</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mima89/looking_for_nyc_nail_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1misjk3</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>fantastic four nails</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyoijkx76bhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1mitfmj</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>I chopped my beautiful nails off, aaahhh!</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mitfmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1mivij4</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Not sure if I like this set</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mivij4</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1mivd0o</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Who's up for something like that?🩷🐄</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/olgldndsvbhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1miv01w</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Summer Nails ~ ☀️ What’s your favorite?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b06ea6r8sbhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1miumft</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Why is it not dry??? 😭</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwboqc2oobhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1miuk60</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>A little summer fun</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miuk60</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1miu6yq</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Just got these done :)</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqd02vinkbhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1mitu0l</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mitu0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1mitkn2</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Purple 💜</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykgs5vk2fbhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1mitd7e</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Chunky jewelry nails!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mitd7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1mit9se</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Finally painted!!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3d55okjfcbhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1mit4au</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Cats eye trial</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4qmdkp4bbhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1miswur</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>I know it’s August but I’m so ready for fall🍄🍂</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8zcm9lc9bhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1misq0d</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>How did I do shaping my nails? Criticism welcome!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugwoarhr7bhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1miso64</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>buying nail stuff!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miso64</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1miskq4</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Unpolished</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okgl8myh6bhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1mis60u</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Is this separation normal?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyeua1s03bhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1mirwm0</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>came back from the dead with a new set lol</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jdevzbws0bhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1mirsr9</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Are these considered good? BIAB extension</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mirsr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1mirqgr</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>DIY Green</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/15agozmczahf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1mipvla</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Tropical Vibes 🏝️</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mipvla</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1mirh22</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>If I get a nail design like this done, should I schedule my appointment as gel or acrylic?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mirh22/if_i_get_a_nail_design_like_this_done_should_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1mir0xr</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Celestial set</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg3jjq1itahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1miqw0a</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Painted my nails on my own for the first time in years. (the white spots are hand cream, lol.)</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miqw0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1miqnuo</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miqnuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1miq3q6</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>i’m obsessed with the set i got today for my birthday!</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ahvdfgzlahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1mipvlq</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Press ons??</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wa391xd6kahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1mipji4</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Cracked acrylic but not real nail. What to do? HELP</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qaiujhihahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1mipdds</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>When life gives you lemons…</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h60fg0d6gahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1miosea</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Favorite set I’ve ever had!</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmvm2p5rbahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1mionu8</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Got my nails done before vacation tomorrow, but I think I’m regretting my color choice. Should I try to get a new color done or be happy with it?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uzoiz2gsaahf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1mioido</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>made my first press on set!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jwa92an9ahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1miofyw</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>❤️🌶️</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7cndig49ahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1miof3c</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>DIY Press ons how to start??</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1miof3c/diy_press_ons_how_to_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1mioets</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Festival nails</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lepc5uhv8ahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1mio04s</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Nail shape opinion</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bt14ufqu5ahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1minjr9</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Help I can't get this off</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbk5jz5h2ahf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1min19d</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>tips for accessible nail maintenance at home?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1min19d/tips_for_accessible_nail_maintenance_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1mimx21</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>What do you think of my wedding nails?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ithpgd9ux9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1mimsvc</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mimsvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1mimoui</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>First time trying round nails (natural)</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mimoui</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1mimjlw</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Christmas is coming 😂</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mimjlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1mime4m</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Ughhh</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mime4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1mim1sg</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Essie blush jelly + chrome powder on top</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep8oqalnr9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1milllf</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Tried gel-x for the first time</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyl54rgko9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1mikl91</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>My first time saying I don’t like my nails!!!!!!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mikl91</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1mikt54</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>first design i’ve done that wasn’t just a copy from pinterest pics! very proud of how far my nail art skills have come (still need to get better at technique but that’s the boring part lol)</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/036355c2j9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1milbqn</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Milky white + chrome</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fsm0ohinm9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1mil0n0</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>embossed pink 💖</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkxskw1jk9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1mikwh6</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>The perfect French mani</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mikwh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1mijqac</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>☯️</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnh908vvb9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1mij2d5</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Getting my nails done for the first time. Last pic is what I'm gonna ask for, but I'd like a fun flair! What would you suggest?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mij2d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1mij8ti</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Press Ons</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mz99zdgn89hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1mij1gq</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Giving nails break from extensions and shellac</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mij1gq/giving_nails_break_from_extensions_and_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1mii3kd</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Maybe the original is new to nails. I hope so</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mii3kd</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1miickk</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>A strawberry set I’ve just finished</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miickk</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1miiut1</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Monet Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miiut1</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1miiw45</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Subtle sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mty4ykv869hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1migxlf</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Safe to Mix Gel Polishes?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1migxlf/safe_to_mix_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1mihix6</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Builder gel question</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mihix6/builder_gel_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1mih1yy</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Lavender mood 🔮</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eio91fr6u8hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1mih0lv</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Tips will be appreciated, first time doing my nails with gelish</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1oaq3lxt8hf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1mifvx9</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>What would you do if the person doing the nails person kept cutting your fingers?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mifvx9/what_would_you_do_if_the_person_doing_the_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1mifg3q</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>wondering if this has happened to anyone else!</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mifg3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1mifamw</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>transition?</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mifamw/transition/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1miergj</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Nail Shape</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlahqc5hf8hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1mif407</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>I bit my gel x off</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mif407/i_bit_my_gel_x_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1miezef</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Walmart nails ❤️</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9stn5kwg8hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1miew0f</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>How on earth can I fix these? (Am desperate)</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xex3chp9g8hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1mieih4</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Calling all Europeans/ Scandinavians, help a girl out💅</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mieih4/calling_all_europeans_scandinavians_help_a_girl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1mieded</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Nails for family member 18th birthday celebration on Saturday 🙌🏼</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mieded</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1mi6y5z</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Why are my nails turning see through?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi6y5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1mi90te</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>What to buy from amazon!</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mi90te/what_to_buy_from_amazon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1mid8nc</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>The bottom “corners” of my nails (Gel X) always seem to be bulky and eventually lift and just look….not very nice as my nails grow, no matter who does them. What do I ask for to avoid this in the future?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mid8nc</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1midrr1</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>80’s Love</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad6m1r1y88hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1midj7i</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>💅🏻💕hi, Barbie!</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1midj7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1mid3av</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Nice design</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2em00ie48hf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1mid3ap</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Can nail techs safely remove acrylic?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mid3ap/can_nail_techs_safely_remove_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1micyxs</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Pusheen nails!! ( ´∀｀ )b</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2k0ru0xi38hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1mictc6</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>/sigh</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mictc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1mib7x9</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>My very amateur summer nails!</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mib7x9</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1micc59</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Nail design I did on my Dad :D</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1micc59</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1micbd9</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>What I wanted vs. What I got</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6y11s0ty7hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1mic3xr</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Musical Nails - First time doing my nails by myself</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mic3xr</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1mibtj8</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Suggestions?</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psphre6jv7hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1mibrg9</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>guys I be having too much fun</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4prhzn5v7hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1mibpn6</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>nails ✨</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eye2toasu7hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1mibkao</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Cutting long, natural nail</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e4brjo4tt7hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1mibik9</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Sunset🌅</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55ra2nbit7hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1mib9js</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>1 year ago Vs now</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mib9js</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1mian1q</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>(19F) I had bitten my nails for 18 years, stopped a few months ago. What do you think of the progress?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mian1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1mi9ku6</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Reputable 3d press on nail makers?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mi9ku6/reputable_3d_press_on_nail_makers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1mixwm9</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Best regular nail polishes</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mixwm9/best_regular_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1mixvsf</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Blue with Pink/Orange Shimmer</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mixvsf/blue_with_pinkorange_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1mixouu</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>New Brand Intro - Aura Bloom Polish (NOT MY brand, just passing the info on!)</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6zr5gz8s7hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1miwrak</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Bugs in amber style nails??</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1miwrak/bugs_in_amber_style_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1miwqar</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Less is more 🤍✨</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ci1xjyt9chf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1miwn5e</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>I broke a nail and had the perfect excuse for a whole different look</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1ij2yw1w8chf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1miwabz</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Careful traveling with your polishes... 😅</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miwabz</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1miw9z6</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>New and Old</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miw9z6</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1mivz3g</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>The living won't usually see the dead</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mivz3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1miv8z0</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Lights of Valinor 🌳</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ydhan2oubhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1miu9nw</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>This color reminds me of blue skies and a nice beach</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miu8qb</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1mitz32</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Tree frog mani while we still have sunshine</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sea1geenibhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1mituxy</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Clionadh mystery polishes</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4yzouu3mhbhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1mitehv</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Y’all… Who did this?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fsbt0nckdbhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1mit4d0</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>bkl skittle on a whim</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nul8vhz4bbhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1misssc</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>cat themed stickers (w/ cat tax lol)</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1misssc</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1mis9qb</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Neon green and holo!!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/464ggwyu3bhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1mirir5</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Joining the PPU train</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mirir5</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1mir9it</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Is this a good nude shade for me?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzcvrwhgvahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1mir984</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>polishes like deep space?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mir984/polishes_like_deep_space/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1miq8u9</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Tried something different!</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miq8u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1miq8d6</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>No longer including mixing balls?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1miq8d6/no_longer_including_mixing_balls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1miq4hh</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Regular velvet vs glass bead effect</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ulj8tc35mahf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1mipu4o</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>"Milk Nails" or "Your Nails But Better"?</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcy81pnujahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1mipjm0</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>2024 summer fruit nails</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mipjm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1mipf7h</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Glass Bead Successful Failure?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6et94n9kgahf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1mii4qs</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Help - shade match?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z02g3e0619hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1mim8cm</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Finally exploring gel polish!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58q54sews9hf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1mip3m8</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>zodiac nail wheel 🌬️🌊🔥🌳</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mip3m8</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1mip080</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Does anyone have this? How do you use it?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v92jsu0edahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1miomld</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Cuticles and organization</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ndpwrs3jaahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1minxv4</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Shadow Daddy</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sk9syua75ahf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1mino7s</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>10 finger skittle</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mino7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1minb93</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>LF Dupe for Holo Taco - Orange Drink</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltr1jeeq0ahf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1mimnq6</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>air sign nails ♒️♊️♎️🌬️</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mimnq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1mimmhw</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Sour Apple Rings screams radioactive slime (in the best way ✨💚)</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mimmhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1milugd</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>What I wore last week</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1milugd</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1miltrw</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Please help ID OPI color</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miltrw</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1milt0y</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Dupe for Sakura's Serenade?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orfjefqyp9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1milmqt</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>i usually hate gold on me but…</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1milmqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1milmki</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>i usually hate gold on me but…</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1milmki</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1mila1n</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Fun fact: Sour Apple Rings can be used for stamping.</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mila1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1mil5s6</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Advice for wedding nails</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mil5s6/advice_for_wedding_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1mil4bz</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>I AM AN APPETITE</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ee2h1l48l9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1mikbc0</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Looking for storage</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmpri21rf9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1mijlyq</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Crown of Wildflowers</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mijlyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1mij9lz</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Healing Waters💙🌊</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqcaelas89hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1miitdw</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Stick insect feat. ILNP Hypnosis</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4z9chi959hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1miijau</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>I need help 😭</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0quwuxjw39hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1mii5bm</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>I am in loooooooove</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mii5bm</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1mihtzm</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>My first PPU purchase</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bldbh9f9z8hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1mihhjw</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Sparkly jelly ❤️</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mihhjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1mifubt</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Better quality dupe of LA colors “exposed”?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mifubt</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1miftsv</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Holo Taco Coral Chaser</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bue4g1pbm8hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1mifnur</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>How are my nail beds?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgl106a5l8hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1mife8j</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>This is me right now</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87v2h4fjj8hf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1mifd1e</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Stabilize a nail bed break?</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mifd1e/stabilize_a_nail_bed_break/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1miexff</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Cuticle disappearing</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqijumbjg8hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1mievmm</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>When you find the color you're looking for on sale 😊 🍉🍎</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smfn3gy6g8hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1miekvf</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Quite Literally Obsessed</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miekvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1miego4</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Primer and base coat? General questions.</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1miego4/primer_and_base_coat_general_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1midicr</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Obsessed with Clionadh</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qnpf0b4578hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1mid8xy</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Moody Beach Nails</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mid8xy/moody_beach_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1mictdz</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Glow in the dark polish</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mictdz/glow_in_the_dark_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1micst1</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>First mani I LOVE</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yuyc3t1b28hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1micsea</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Does anyone else feel an insane amount of indecision paralysis choosing a polish for a vacation or a special occasion?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1micsea/does_anyone_else_feel_an_insane_amount_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1micqk7</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>cyborg french tips</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rabdduuv18hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1mi9uf2</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Adore this combo!</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi9uf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1mi9mq4</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>July Manis 💅</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi9mq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1mi9g9o</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Kpop Demon Hunters</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi9g9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1mi8dxz</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Essie Gel Couture Lack mit Essie treat love and color als Top Coat kombinierbar.</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mi8dxz/essie_gel_couture_lack_mit_essie_treat_love_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1mi80ez</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>What shape nail is best for my long chubby fingers?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1b2jvhy947hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1mi5hqq</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Update! - black light mani</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi5hqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1mi4y64</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>🌺🌺</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi4y64</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1mi3pog</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>PFD Angel Wings</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w45dpss3x5hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1mipgb0</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Girls, do you recommend these gel products?</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xslenaetgahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1miosnb</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>i cant stop staring at the shiny</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xvzwp2tbahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1mim2x0</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>They look even better in real life… the camera doesn’t do them justice 😩</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ak6lqwvr9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1mikyg5</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Kawaii cute nails I did today!</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d37pegb4k9hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1miiwjh</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>What should I put on the ring fingers for this set?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miiwjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1mii9a1</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Green n Gold⚜️💚</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/196s0ww029hf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1miekj5</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>3D effect over cat eye</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miekj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1mici4m</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Tropical Vibes 🏝️</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mici4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1mibfne</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Competition Set for Empire and OPI</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mibfne</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1mia6sb</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Some of the sets I’ve made in the last couple weeks :)</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mia6sb</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1mi8s0z</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Recreated this set by allycoolcattt</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9ynw5b6a7hf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1mi7zr2</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Help with chrome isolation</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mi7zr2/help_with_chrome_isolation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1mi7b91</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Second attempt at stamping, I am really happy with them</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mi7b91</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Aug  7 08:14:22 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_10.xlsx
+++ b/data/collected_data/2025_08_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C707"/>
+  <dimension ref="A1:C907"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12452,6 +12452,3406 @@
         </is>
       </c>
     </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1mju574</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Can UV Nail Lamp be used to quickly dry Nail polish / Nail Lacquer (not gel polish!)</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mju574</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1mjssip</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>adhesive allergy, looking 4 alternatives</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mjssip/adhesive_allergy_looking_4_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1mju00m</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>So proud of my nails!</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mju00m</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1mjqzu8</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>I bought some nail files, but they look off, should I be concerned?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51tjaqn03jhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1mjnubl</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Nature/insect inspired nails!</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjnubl</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1mjo42o</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Had my nails done professionally for the first time</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjo42o</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1mjpigu</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Healthy natural nails with gel</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9l5eg1yoihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1mjp68s</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>tortoise shell and blueberry lemon!</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhufo67wlihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1mjouiu</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>First time doing press ons</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rb8iiqo1jihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1mjop64</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>first post kinda nervous 😳😳</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjop64</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1mjo75u</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>i’m obsessed with press ons</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjo75u</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1mjo6rl</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>My girl did it again 🥰</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg2jxvnedihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1mjo0d0</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Shark Nails</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84vx7jzvbihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1mjnz86</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Ideas!!</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjnz86</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1mjnykl</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>they like</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6830ip0hbihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1mjnqkx</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Lavender Chrome</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjnqkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1mjmpe1</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>I'm in my Mexican folk art inspired nails era</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjmpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1mjng7u</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Are these worth $75?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjng7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1mjn6v4</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Do You like My blue Nails?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3nmw4n25ihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1mjmeyj</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>are these cute? i did them</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cng7paqqyhhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1mjlxr5</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>How to know which size to use and how to prep natural nail before?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mjlxr5/how_to_know_which_size_to_use_and_how_to_prep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1mjlw22</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Am I cooked</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjlw22</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1mjluaf</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>First time getting airbrushed nails for this subtle cotton candy chrome.</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjluaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1mjl0qv</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>When should I get my nails filled in?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjl0qv</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1mjl79q</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Love my French nails 🤍</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjl79q</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1mjkfes</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Screaming bc I actually love them</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctfqnd4wihhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1mjk3g1</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Sunset inspired nails 🌅</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xe6soiscghhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1mjk0cd</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Matcha Nails</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjk0cd</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1mjjusm</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>I would like to brag about the little mani I gave myself last night for a moment</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjjusm</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1mjjsk2</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>RIP my natural nails</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjjsk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1mjjjg8</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>💅🏾 🪴</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/84qdbk44chhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1mjj9ah</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>💜🌸</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxvil8kz9hhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1mjj2e6</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>end of summer nails 💗🧡💜</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwbdeyol8hhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1mjj0au</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Is this almond or oval?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wl85n8468hhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1mjioke</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Does an acrylic overlay usually come with a cuticle trim and am I asking for the correct service?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mjioke/does_an_acrylic_overlay_usually_come_with_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1mjio5z</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>1 month worth of growth, time to repaint! 💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjio5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1mji48m</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>I’m getting better</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mji48m</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1mji8u4</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>I love my new nails, first time posting here</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0uqvztp2hhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1mji5wj</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Favorite gold polish? I like this as a top coat, but I’d love to know what others use!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utcn01x42hhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1mji5gm</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>The ombré is a bit off but I’m quite pleased with the hand painted silhouettes I did on my friend’s nails</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mji5gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1mjh96v</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>back with another one ✨</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dktd6tmrvghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1mjhsun</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Got my nails fixed finally (update from walking out of chop shop)</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjhsun</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1mjhomp</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Naiiilz!!! Rainbows are bringing me all the joy lately- also yes I took this pic with my thighs lol 🌈</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v65dtjqryghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1mjhh0j</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Lifting? Will I be fine to wait till my appointment on Sat.?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyu7iceaxghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1mjhclg</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Had to share H0T PINK &amp; BUTTER YELLOW aura 💅🏻</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjhclg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1mjh0uq</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>My Starfish Nails</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6hcqpk7ughf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1mjgsei</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Anyone else a cat eye fan?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vmd3nphlsghf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1mjgqun</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>new set for myself! is it giving summer fairy vibes?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/apy8l7jasghf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1mjgpr6</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Marshalls coming in clutch</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2iutwe3sghf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1mjgnsk</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Dip Powder Question</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mjgnsk/dip_powder_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1mjgf1l</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>wth is on my hands?? inspo from @preppyclick on pinterest</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjgf1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1mjgbln</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>fish and oysters!!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjgbln</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1mjfj9o</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Does a full set ever come with “manicure” services?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mjfj9o/does_a_full_set_ever_come_with_manicure_services/</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1mj4bjd</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Best products/routine for long lasting at home acrylics?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mj4bjd/best_productsroutine_for_long_lasting_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1miw2ez</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>UPDATE: Thick Nails. AIO??</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miw2ez</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1mjfdip</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>my first ever set of press ons!</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j84wzjzuighf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1mj7uo7</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>anyone know a true brown red nail polish like this?</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yck3qjqf4fhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1mj9us3</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Help! How can I make my nails look good?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tfbnygshfhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1mjazuj</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Crack in nail</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62e0erpcpfhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1mjbm7y</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Probably my last time getting my nails painted :(</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8ktj14htfhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1mjbu87</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Uk good nail polish brands?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mjbu87/uk_good_nail_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1mjcsyw</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>I have the best nail tech</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjcsyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1mjf95d</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Take me back to the 2000s</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmrfl8a1ighf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1mjf003</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>how much?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjf003</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1mjeq0i</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>my friends first nails!!</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgoz6dwfeghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1mjelgz</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Rawr 🐯</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7re8dokdghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1mje7cg</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Acrylic or BIAB for pedicure?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mje7cg/acrylic_or_biab_for_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1mje5ke</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Zero file / sin limado semi - gel nails</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q94jia8iaghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1mje431</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Update: got them fixed (don’t mind the light reflecting lol)</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mje431</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1mjdy3z</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Russian mani —&gt; gel</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mjdy3z/russian_mani_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1mjdq18</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Nail biter that can't keep nails on</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mjdq18/nail_biter_that_cant_keep_nails_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1mjdnin</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>End of Summer Nails</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6ek60d47ghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1mjdn6v</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>My nail tech has truly learned my vibes.  Freestyle appt.</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kk7gt4127ghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1mjc7al</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>New set💅🏾</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjc7al</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1mjc79i</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Just got the worst and most rushed French tip of my life bro 😭</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjc79i</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1mjc70g</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>how have you saved your brittle nails?</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mjc70g/how_have_you_saved_your_brittle_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1mjc536</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Conference Nails</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lut1442xfhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1mjb3bq</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>🍄👽🛸✨</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjb3bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1mjapnr</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Skinny Fingers, Narrow Nailbed</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mjapnr/skinny_fingers_narrow_nailbed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1mjac0u</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>citrus nails 🍊🍋🌸</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjac0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1mja083</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Getting a fill weekly?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mja083/getting_a_fill_weekly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1mj9yuk</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Cali nails</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqizhagkifhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1mj8ui7</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Question about hard gel</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mj8ui7/question_about_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1mj7uts</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Looking for a Veil or Blush polish</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mj7uts/looking_for_a_veil_or_blush_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1mj7u49</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Can gel x be shortened?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6wmumnb4fhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1mj7s1t</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>After years of nailbiting I finally love looking at my hands ✨️</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukb69bbx3fhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1mj7a9x</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>How to take off top gel/polygel nails + gel?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mj7a9x/how_to_take_off_top_gelpolygel_nails_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1mj6wd9</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Perhaps a stupid question, but how do y’all keep your nail oil from transferring on things??</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mj6wd9/perhaps_a_stupid_question_but_how_do_yall_keep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1mj6k9s</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>LED lights</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mj6k9s/led_lights/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1mj5m1b</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Family/friend clients</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mj5m1b/familyfriend_clients/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1mj5kn7</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>First time doing ombré (and posting here)</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj5kn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1mj5epl</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Polka Dot Nails 🤍</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbcl0ukonehf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1mj3at3</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Vacation nails!!</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj3at3</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1mj4nco</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>My nails for waiting to find out baby’s sex 🩷💜💙</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1act31tyhehf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1mj3hov</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>I’m confused with all the options</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mj3hov/im_confused_with_all_the_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1mj4pwq</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Opinion needed: are these nice? (Shellac)</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj4pwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1mj4lzk</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>love these polishes</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj4lzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1mj4kvt</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Broke the acrylic on top of my real nail last night. Can’t tell if there’s a small crack in my actual nail 😭</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9rdub7mghehf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1mj4jn7</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>I just wanted to show off my nails</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgdg1au6hehf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1mj4ari</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>UV gel removal - what to expect?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mj4ari/uv_gel_removal_what_to_expect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1mjsaw3</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>don’t sleep on this $3 poparazzi polish</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjsaw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1mjs5hs</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Neon Corals??</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mjs5hs/neon_corals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1mjr2xh</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Here is my latest attempt at painting some nice stuff on my nails. I'd appreciate some tips or feedback (more questions in the description)</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjr2xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1mjqr8i</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>New to this in the last couple of weeks.</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjqr8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1mjqqb3</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>What color could be close to this?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57m8yy9h0jhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1mjpr1w</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Shade recs for this eyeshadow turned watercolor?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bm0rqctsrfhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1mjphbw</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Mixing magnetics</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/57m3fvpnoihf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1mjp8fz</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>How can I stop my top coat from making my nails bubble 🙏</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jqc8ej5mihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1mjnqo1</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>New glass bead method</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lp43hkbm9ihf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1mjmx50</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>This polish smells like jelly shoes</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5af0nd9v2ihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1mjmu78</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Jumping on the Glass Bead Wagon!</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjmu78</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1mjmqjz</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>What are your favorite top coats?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulx3do4c1ihf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1mjlmi7</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Freebie Product Question</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjlmi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1mjkmhd</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Creative ways to stop biting/picking?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mjkmhd/creative_ways_to_stop_bitingpicking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1mjkkhj</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Finally got my space set up!</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjkkhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1mjkce4</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Day 7 of my mani, including 3 nights of camping and 2 full days of mountain biking</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjkce4</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1mjjlgr</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>What are some polishes that look like this beetle in my backyard?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjjlgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1mjiuqg</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>I am so ready for autumn 🎃</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjiuqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1mjiboq</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>I call this tennis ball ecoplasm</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjiboq</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1mji6vd</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Which brands have good rewards programs?</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mji6vd/which_brands_have_good_rewards_programs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1mji3cq</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Made my first set of press ons 💙</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mji3cq</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1mjhitl</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>just got ILNP storm watch &amp; I’m so excited to pair it with flicker 🤩</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n8msy6amxghf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1mjgspg</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Gotta love a shifty shimmer!</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sj2i4wgsghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1mjgrpu</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>ILNP Sabrina 💅</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qy0msrrtrghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1mjg4r4</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Colors like Essie Bodice Goddess?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mjg4r4/colors_like_essie_bodice_goddess/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1mjfh2h</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>green cremes 4ever</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f84lzycijghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1mjf6b9</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>I may have peely based too close to the sun</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjf6b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1mjeztt</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>i love l.a. colors</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjeztt</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1mjeo48</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Unconventional base coats?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mjeo48/unconventional_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1mje5og</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Polished for Days What Was I Made For?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mje5og</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1mje2qi</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>What on earth is happening?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mje2qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1mjdo7z</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Flower Child, cult favourite</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwo7q5x87ghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1mjdku0</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Psilocybin help!</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjdku0</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1mjdglm</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Getting Back into actively painting my nails again, so I bought a ton of new polishes and arranged them to look pretty!</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j12f7m9u5ghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1mjcrhs</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>High Roller</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n56b1a071ghf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1mjcc74</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Sprite Nails! 🍋</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ap9ek81fyfhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1mjc4nw</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Looking for a lavender sky dupe</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mjc4nw/looking_for_a_lavender_sky_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1mjc49x</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Simple summer nails 💙</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjc49x</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1mjc2q6</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Late July Mani's</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgs9tzolwfhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1mjbcrr</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>My birthday nails! Cupcake Polish - Funfetti</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjbcrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1mjasq0</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>I went to a crayfish dinner last night 🦞</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjasq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1mjarut</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Color theory</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mjarut/color_theory/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1mjakwk</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Got these today. Anyone know when they were released?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2iowl74lmfhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1mjai0y</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Feo, Fuerte y forma dupes please!</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mjai0y/feo_fuerte_y_forma_dupes_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1mjad8g</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>How to beautify your office supplies</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnhdugj6lfhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1mjabp1</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Finally changing my brushes.🥲</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ic1ngvuwkfhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1mja5q4</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>How often do you repaint your nails?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mja5q4/how_often_do_you_repaint_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1mja19t</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Pregaming for fall with this thermal</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1v0zs90jfhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1mj98id</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Pink lemonade look 🍋 🩷</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj98id</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1mj91lu</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Concert Nails</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/019758decfhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1mj8zsi</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Help! Deep break happened at work. Anything I can do to make this last until I get home?</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgpbwh62cfhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1mj8ut8</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Soot Sprites for a Bday Mani</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj8ut8</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1mj8tsf</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>This is 8 months of not biting my nails and this is what I have to show for it. Can you tell which hand I use the most?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj8tsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1mj8qsl</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>First Bee's Knees order</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gids51idafhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1mj86vu</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Jelly skittle</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj86vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1mj80o5</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>I hate my lumpy, bumpy thumbnails</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qkojabk5fhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1mj7ulc</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Polished for Days' Blossom and Eternal Glow: comparison</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj7ulc</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1mj7sm4</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>ILNP Aerial View perfectly matches the water in Glacier National Park, Montana</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj7sm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1mj7o2o</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Are yall sick of my mom’s manis yet?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwdizzk83fhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1mj7lnm</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>First time doing the velvet effect! (Penelope Luz: Butterfly Wings)</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ussg6xhx1fhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1mj6t1y</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Trying to be an ✨ elegant ✨ lady</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj6t1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1mj6a81</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>I feel like I've tried everything</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z59ccz1vtehf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1mj69bg</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Day 9 and I don’t want to take it off 😩</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5rgc8ccotehf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1mj5t1w</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Cirque - C'est Chic (Merkitten dupe?)</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5eyz4w9hqehf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1mj4ktq</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Okay, y’all made me get my first magnetic polish. Looking for magnet recommendations now!</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mj4ktq/okay_yall_made_me_get_my_first_magnetic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1mj4as3</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>It’s my turn, y’all are wonderful and terrible</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tals9qw9fehf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1mj3uwr</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Very new to this!</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nw39aic1cehf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1mj3um8</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>High Tea Hibiscus and Cosmic Unicorn Skin</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj3tss</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1mj3ram</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Cuticle care, and a question</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj3ram</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1mj3gfo</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Anyone here who owns Jack Frost by Vanessa Molina?</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mj3gfo/anyone_here_who_owns_jack_frost_by_vanessa_molina/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1mj3alo</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>friends, how are we painting our toes?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mj3alo/friends_how_are_we_painting_our_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1mj35z1</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>PFD Limelight</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l37c463d6ehf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1mj2kvj</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>First time doing at home gel on my natural nails!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj2kvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1midsfc</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Well, I repurchased the suspected fake Opi direct from wellastore this time, and they look even more confusing, so I guess they weren’t fake?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1midsfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1miozdi</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>First post! Love micro shimmer so much</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llkev1v6dahf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1miraho</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Another semi-unhinged magnet DIY</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jph9lyonvahf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1mj08q5</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Death Valley Nails</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mj08q5/death_valley_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1mj07yf</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Magnetic Polish and Top Coats?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mj07yf/magnetic_polish_and_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1mizjl9</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Tried glass bead effect, I like it!</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w49d8z936dhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1mjsbnc</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Pink glitter nails with rhinestones</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5u32mky9gjhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1mjro1y</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>nails I did last year</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjro1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1mjpzsq</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Cherries!</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjpzsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1mjpz0z</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>design advice</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6j8jzd9tihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1mjp5pc</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>tortoise shell frenchies and blueberry lemon nails !</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8f47sfrlihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1mjodwx</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>pinterest inspired</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjodwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1mjnlfl</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>They like?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wvhqkmf8ihf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1mjmuki</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>creepy nails</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjmuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1mjmnqs</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>I can't stop doing Mexican folk art inspired nails</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjmnqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1mjlr86</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Gel cat eye polish that doesn’t need a base color?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mjlr86/gel_cat_eye_polish_that_doesnt_need_a_base_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1mjl5nv</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>First ever press on set 💖</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjl5nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1mjk1ch</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Back to school nails 📕📕</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3ee9lkwfhhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1mjjak5</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Nostalgic 90s</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v16lng09ahhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1mjjagd</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Nail inspo help</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjjagd</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1mjiyqv</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Aurora effect nails🤍</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxf5xbtu7hhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1mjhmwg</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Shark Nails</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhthbapfyghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1mjg8os</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>I love this effect on the nails, it's called cat's eye</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbf8viktoghf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1mj5wtu</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Silver foil and rhinestones</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtahveo4rehf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1mj0phd</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Air bubbles under cured gel polish/gel</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjjyl0b1jdhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1mj0cxn</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Cherry and blueberry pie nails :)</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mj0cxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1miiw9y</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>💅🏻</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1miiw9y</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Aug  8 08:14:05 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_10.xlsx
+++ b/data/collected_data/2025_08_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C907"/>
+  <dimension ref="A1:C1095"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15852,6 +15852,3202 @@
         </is>
       </c>
     </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1mkp2lr</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Celestial Gel-X DIY</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imh0qb153rhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1mkoqoe</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>I’m new to gel nail gels - are these lifting?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkoqoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1mko9z8</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Definitely my new go to nail color. DND #458 -fresh eggplant</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uc3t4d4uqhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1mko9rq</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>LOVE my star✨ nail art</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vveey50uqhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1mknyyq</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Today's work, I liked them!</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vss9utpqqqhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1mknybr</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Love my nail tech</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mknybr</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1mknk05</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Am I nails blind</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mknk05</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1mkn658</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>First time with long, fancy nails!</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfhz8c7aiqhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1mkmyt6</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Trying nail art on myself for the first time in years!</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkmyt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1mkm31h</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>How do you get anything to stay?</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkm31h/how_do_you_get_anything_to_stay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1mkkyqr</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Nail Etiquette/Disappointed HELP!</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkkyqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1mkms1o</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>How should I deal with this partial break? My wedding is in three weeks :)</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/016586w3eqhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1mklv9z</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>My wedding nails. I'll post an update when I add gems tomorrow.</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mklv9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1mkl2l8</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>How did my nail tech do?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/insy1jenxphf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1mkl1d1</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>What do you all think?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkl1d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1mkh7du</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>happy with how these came out!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kwoux8bzohf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1mki6i3</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>My nails in June vs my nails now</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mki6i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1mkjntc</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Felt cutesy</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkjntc</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1mkjl8u</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>shiny &amp; bright ✨</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkjl8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1mkje4f</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkje4f/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1mkjbj4</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Who prefers regular polish over gel polish? Or visa versa</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkjbj4/who_prefers_regular_polish_over_gel_polish_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1mkiw16</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Cutesy Nails!</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lurnnfn6ephf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1mkioch</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Summer blues 🌊🦋🐬</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkioch</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1mkigsb</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Birthday Nails ❤️💋🥰</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qspjslolaphf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1mkicso</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xdisl24o9phf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1mkicqx</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Why do they look like this ???</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkicqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1mki72e</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>are these good for nails ?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mki72e</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1mki38x</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>I have a confession to make : Matching red fingers and toes make me feel more confident. ❤️</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9lwy3xe7phf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1mkhaaz</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Gel Polish Curing Time</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkhaaz/gel_polish_curing_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1mkh9xe</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Too long?</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mx092v2m0phf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1mkgi0s</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Tomatoes</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkgi0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1mkgdi5</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>First time doing acrylic nails on someone!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xki4r7e6tohf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1mkg4w1</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>I love my nail tech 🥰</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnzigzd7rohf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1mkftp0</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>How to use these foils if I don’t have the products stated on the back?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkftp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1mkfjyt</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>What should I change?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkfjyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1mkf3pe</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Are these acceptable?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkf3pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1mket90</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Chrome-y goodness in the backcountry</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mket90</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1mkcqlg</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Super dry nails, how to help?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkcqlg/super_dry_nails_how_to_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1mkcqr0</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>My gel nails feel soft?</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkcqr0/my_gel_nails_feel_soft/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1mkd3jy</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>My current nails</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkd3jy</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1mke8uc</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Would it be rude to ask the salon to file these more?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mke8uc</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1mkbzq6</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Made press ons for the first time! (and second time doing own nails)</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci04avscwnhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1mkbtax</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>What’s the best type of polish/technique for growing and strengthening natural nails?</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkbtax/whats_the_best_type_of_polishtechnique_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1mkbd6n</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>What do I do with this nail?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/csw50z81snhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1mkbhho</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>I keep staring at my nails instead of doing work lol..</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/89s3zwwtsnhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1mkbhif</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Rodeo nails 🐎</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrm0zgpusnhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1mkb7ov</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Ideas for formula 1 nails</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkb7ov/ideas_for_formula_1_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1mkae69</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>help with shape!</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtxrnevdlnhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1mkabgi</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Is the burning normal?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkabgi/is_the_burning_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1mka0wx</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>~ Cha-La HetCha-La ~ @v.rnish</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqjx3u7vinhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1mk9tl6</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Dark green pedicure</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk9tl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1mk9j1r</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Sometimes painting my natural length nails is a breath of fresh air after having extensions</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3sja3hhfnhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1mk9c06</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Strengthening advice!</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mk9c06/strengthening_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1mk8x97</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>What is this?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nen9e2kcbnhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1mk874z</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Too neutral?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zie6elvg6nhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1mk7zrk</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Prepping for my first market!</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk7zrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1mk80lh</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>my sister’s clean girl nails😌💅</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk80lh</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1mk7rlr</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Gel X at home</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mk7rlr/gel_x_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1mk7gr0</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>first time ever getting gel x</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk7gr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1mk5ylc</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Gel Manicures😍</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk5ylc</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1mk41ls</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>What do I ask for?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4k5y461qemhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1mk0nbj</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>💭 What’s your dream nail set right now?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mk0nbj/whats_your_dream_nail_set_right_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1mk6lxq</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time in 6 years and the nail tech cut 3 of my fingers in the same spot</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk6lxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1mk6qn5</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Lifelong nail &amp; cuticle biter - what finally helped you break the habit?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mk6qn5/lifelong_nail_cuticle_biter_what_finally_helped/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1mk6xzx</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>is this normal?</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk6xzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1mk5rui</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Can anyone help identify this shade Kylie Jenner is wearing?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itwg9tzaqmhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1mk5zeb</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Nail art for trip to…</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mph4i2pmrmhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1mk52yp</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Bold nails!</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk52yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1mk4hos</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>How cute are these press ons 🐸🍄🍒</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk4hos</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1mk3xrg</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Beginner set of tools?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mk3xrg/beginner_set_of_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1mk3ofn</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>nails for august!!!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3mnjiwacmhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1mk32lg</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Nail Art with Dazzle Dry?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mk32lg/nail_art_with_dazzle_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1mk2g7l</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>what’s wrong with my nail?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4oq84rwx3mhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1mk24ib</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>First time doing Gel X, Looking for Critique!</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk24ib</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1mk1g0j</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Damaged Nails Question</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/row1ppnzwlhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1mk115i</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Was it beautiful?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v05lyf51ulhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1mk0h3f</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Biab removal after 2 years</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk0h3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1mjzus8</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Trying nails for the first time 🥰💅🏻</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjzus8</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1mjzrpn</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>favourite nails i did over the years</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjzrpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1mjz0zq</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Do i have short nail beds?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5go2dj0flhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1mjyzy2</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Halloween all year round for me 🖤</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fgirw9selhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1mjxrnn</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjxrnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1mjx92n</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>How to stop life for real?!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjx92n</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1mjx7et</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Press on nail sizing?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mjx7et/press_on_nail_sizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1mjwaz4</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Is a space between real nail and bio gel nail normal?</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjwaz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1mjvsba</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Do you like my latest design? 😍💕</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjvsba</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1mjvdtp</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Devastated</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcomwukifkhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1mjux72</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Did my own nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjux72</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1mjuo89</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Nails with ducks!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4minyb9c7khf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1mknv2r</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Colores de Carol - Wavelength</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mknv2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1mknqst</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>I've got an obsession...</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mknqst</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1mkn51f</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Pokémon from Mundo de Unas</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkn51f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1mklwj8</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Yay or Nay?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58zuevbe5qhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1mklq5x</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>The Most Venomous of Octopuses: Good Polish Inspiration?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mklq5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1mklais</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Even safer contraption, glass bead effect tested</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2ur1kpcmzphf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1mkl1wx</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Gimme your most unhinged ways to temporarily "glue" on press ons</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkl1wx/gimme_your_most_unhinged_ways_to_temporarily_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1mkl07p</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Magnetic viewing film</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkl07p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1mkkmho</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>My fave technique with shimmers - mother of pearl 🦪</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9kjlqfknqphf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1mkjbaf</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>man down 😔</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s08cit5thphf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1mkig6n</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>I made Nezuko Demon slayer nails using eyeshadow 😄</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkig6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1mkh9o3</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>I’m in love</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p694zanj0phf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1mkgmzn</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>How can I keep my pointer and middle nails from bending?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyh6ohsdvohf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1mkgj1b</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Base Coat Under Press Ons?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkgj1b/base_coat_under_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1mkgcn6</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Best solar polish top coat?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkgcn6/best_solar_polish_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1mkg7e3</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>First August Mani</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkg7e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1mkg50c</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>22 hour update on new glass bead method</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j7qv5vv7rohf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1mkg2r4</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Pier Perfection</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkg2r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1mkfz4i</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>New to DIY dip nails and nail art, and I'm loving it!</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkfuac</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1mkevei</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Accidentally stuck my fingers into a fan...RIP my nails 😭</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mux6fq7bhohf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1mkei05</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>1st attempt at velvet nails. I'm not sure what I think. Does it look like it's supposed to?</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkei05</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1mkefbs</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Blurring base coat or nude cream?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0fqifywdohf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1mke91e</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Does anyone else go mad scientist with the magnets?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mke91e/does_anyone_else_go_mad_scientist_with_the_magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1mkdjqc</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>What nail polish color for this bridesmaid dress</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqb0n5lc7ohf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1mkdiky</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>You know it's bad when you can smell the polish before you open the mailbox</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkdiky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1mkcuyb</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>It’s me, a woman in stem</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ym7hi78e2ohf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1mkcma8</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>KBShimmer base coat order?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkcma8/kbshimmer_base_coat_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1mkbbz0</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Jelly Polish Bundle Recs?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkbbz0/jelly_polish_bundle_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1mkb9u2</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>ILNP After the Rain - cool colors skittle</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkb9u2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1mkb0q6</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Another Glass Bead Set Up</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/73k0pxmipnhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1mkavn1</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>My First ILNP Order!</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvg7vfeponhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1mkasvd</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>first time trying the glass bead effect. it’s so magical</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z9658tn5onhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1mkahej</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>My first Emily de Molly polish 🔥🪐✨</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7cfd18s0mnhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1mka7k7</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Playing with my stamping plates and old polishes</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mka7k7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1mka709</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>🧡 Prugly Fall Skittle 🍂</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mka709</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1mka4d2</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>So, how long do your magnetic manis take?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mka4d2/so_how_long_do_your_magnetic_manis_take/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1mka3n9</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Yall I just discovered nail stickers and now idk if I’ll ever do a mani without them again 😍</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mka3n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1mk9yoj</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>pinkie pie inspired &lt;3</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekatzrruhnhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1mk9wp6</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>LICHT IT UPP</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dsv27j8chnhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1mk98ac</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Help me pick a polish to match this dress!</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk98ac</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1mk8zdh</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Reciprocal gradient</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk8zdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1mk8m49</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Swift &amp; Saddled🪲🩵</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk8m49</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1mk8c7i</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Matching with my beloved emotional support waterbottle!</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk8c7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1mk8b1a</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>A mid summer set</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sphtqnq67nhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1mk894e</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>A dupe for berry tempting?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2g48hbu6nhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1mk85t1</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Redemption - poesidon's prize</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19y41t976nhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1mk7rf0</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Opi comparisons：same shade, different line.</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk7nb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1mk7ocu</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>cat nails inspired by another laquerista (plus cat tax obvs)</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk7ocu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1mk7o34</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Was jealous of all of your neons</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0k2rs33w2nhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1mk7e3g</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>natural nails holo taco one-coat black</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2ubctac0nhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1mk73r4</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Yay, paddle brush! ILNP Comet</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mk73r4/yay_paddle_brush_ilnp_comet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1mk6zwo</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>What's your favorite dip base?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mk6zwo/whats_your_favorite_dip_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1mk6pn9</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Lifelong nail &amp; cuticle biter - what finally helped you break the habit?</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mk6pn9/lifelong_nail_cuticle_biter_what_finally_helped/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1mk6hj2</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Fiery orange!</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk6hj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1mk694b</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Looking for the perfect galaxy polish</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdoria69smhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1mk61o4</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Favorite Lavender/Lilac polish?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqrtu983smhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1mk5q7u</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Birthday Nails 💅 🎉✨</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk5q7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1mk5jmo</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Cirque - Showgirl</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk5jmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1mk5h12</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Helppp!!!</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mk5h12/helppp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1mk5fan</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Angel Wings dupe!! + cat tax</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ibi4u7o4nmhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1mk59kd</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Where do you get supplies from? Magnets, tools, etc.?</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mk59kd/where_do_you_get_supplies_from_magnets_tools_etc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1mk4kxy</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>dollar tree finds!</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tllfybxbimhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1mk47wh</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Help replicating this color combination</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1w4sc3wfmhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1mk40m3</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Jelly glitter gradient 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guqvm1wkemhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1mk324y</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Some of my nail looks from this last week. Which colors are your favorite?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4hma8th28mhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1mk2gs7</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Finally tried the one and only magnetic in my collection.</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk2gs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1mk1yu7</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Twice in a blue moon</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk1y8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1mk1omw</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Essie has my whole heart 💚</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/364csb3nylhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1mk1bzu</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Lone Star Rose</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk1bzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1mk0zoz</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Bog Dweller and Glass Bead were made for each other</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ksnzmibotlhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1mk0ky4</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>blueberry lemon nails</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fy53ygrqlhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1mk0gch</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>my nails for the Lord Huron concert tonight!</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/prvztw3tplhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1mk0eh3</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Want to do a new mani, want to keep current mani forever…the struggle is real</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2340fpleplhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1mk0b0b</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Pain in the Asteroid 2.0</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tt3bslkmolhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1mjzvfb</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Dupe request: Orly Cool Cucumber from 1998</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DCFfP4sONaX/?igsh=ZTFid3M4ejR2cHZ6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1mjzanw</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Just some simple little soap nails 🧼</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fc1wxie4hlhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1mjyxuy</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>First post ~ 404 soul not found</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vg63rjp8elhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1mjxyzq</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Grungy glitter</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mjxyzq/grungy_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1mjx5v6</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>First Vinted haul + cat tax</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjx5v6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1mjv8ld</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>How do I avoid these bubbles? Please it's been annoying me for ages😭😭😭. All the tips I've tried didn't work reliably and there seems to be no reason why they appear sometimes.</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oh85xrqvdkhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1mjubah</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>My new cat manicure. Love it!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bfsy4co2khf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1mkmwdz</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>I tried doing nail art on myself for the first time in years…</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkmwdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1mklw0a</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>I love cat eye</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k5q54195qhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1mkljxo</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>First time here, I love teaching this art, we love this cat's eye polish and wine base</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7wdgcc22qhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1mklc5y</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Today's work, I really liked it, would you change anything?</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8dge3420qhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1mkk7st</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Seashell Nails 🌊 🐚</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkk7st</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1mki5i4</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Madam Glam First Impressions!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mki5i4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1mkhcza</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Nails I made today</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3k0qmzjb1phf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1mkf7br</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Finally tried blush nails, can't get the picture to show them right but they're beautiful in real life. They're much more pink irl.</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkf7br</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1mkf36u</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>New to DIY dip nails and nail art, and I'm loving it!</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkf36u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1mkevpc</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Mariposa 🦋</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k44wztedhohf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1mkead4</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Sugar, spice, and super cute nails ✨💅💥</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/921rdsoucohf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1mkcchb</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Under the sea for Leo birthday</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkcchb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1mk7w97</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Is it me, or should I change something?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lq4rpg9e4nhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1mk34lj</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Doing my own chrome</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk34lj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1mk23lb</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Matte Flowers, Hybrid Gel</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk23lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1mk0g67</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>my shark nails!</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mk0g67</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1mjw629</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>I was quite pleased with these hand painted silhouettes I did on a friend last night</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mjw629</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1mjw4j4</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>*dead*</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DM86SVtOU6k/?igsh=Y3FwY3NqZjJ2a3pw</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Aug  9 08:11:38 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_10.xlsx
+++ b/data/collected_data/2025_08_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1095"/>
+  <dimension ref="A1:C1310"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19048,6 +19048,3661 @@
         </is>
       </c>
     </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1mljn5u</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>I love silver nail polish so much</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pspaeyx96yhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1mlje2i</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>What is the safest and most affordable way to get your nails done?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mlje2i/what_is_the_safest_and_most_affordable_way_to_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1mlih8o</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Help me switch to Almond nails?</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mlih8o/help_me_switch_to_almond_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1mlgbf6</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Hyper realistic gel x</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x91xp9tp6xhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1mlh824</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Nails I did on my sister</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc8xetvnfxhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1mlgcz6</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>My GF is in school to be a nail tech and needed a client for today i volunteered 🖤 💅🏿</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlgcz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1mlfyys</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>My favorite color :)</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzmf3x1a3xhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1mlfnq6</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>The #1 Reason Why : Boys should paint their nails. Look How CUTE 🩵</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iy42s7rk0xhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1mlf5ut</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>My Ozzy tribute nails 🖤</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlf5ut</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1mld92q</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Long stick glitter nail polish??</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ll4i2en0fwhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1mlecpo</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>first time using poly gel</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lh4p4emowhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1mldn05</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Should I remove the gel manicure I had done today?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mldn05/should_i_remove_the_gel_manicure_i_had_done_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1mlebyi</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Q for anyone who does nails:</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nodu3uffowhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1mlebnr</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>3D Gel practice</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlebnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1mle3q0</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Super proud of my latest set 😊</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mle3q0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1mldy8x</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Nada mal para una primera vez</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2eq95h72lwhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1mldl93</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>finally change the color</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qx51gb2zhwhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1mldk10</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Repainted them, still long as ever! A little over 1 month progress.</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mldk10</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1mlb2fs</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>How to keep shellac staying?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlb2fs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1mlbzz5</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>My first try at gel nails 🌸 They took SO long lol</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgrl8hn44whf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1mlahso</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>How bad are my nails?</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlahso</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1mlai5w</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>I found decent press-ons for longer nail beds!</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlai5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1mlbrtd</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Second time doing gel nails, how did I do?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlbrtd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1mlb04q</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>The Assignment is: Geometric</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlb04q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1mlawy6</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>My first time having long nails in years!! Underneath is a horrible bitten mess</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlawy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1mlaj0v</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>I loved them 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8lvqdg4svhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1mladal</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Lava Goddess 🔥</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pva911nuqvhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1mlabls</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Nail shape to rounded?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlabls</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ml9yzf</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Pink nails</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crvduak4nvhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ml9sg2</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Butter yellow 💛</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml9sg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ml9njx</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>New to DIY dip nails and nail art, and I'm loving it!</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml9njx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ml9nem</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Nail Care and timing of re do</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ml9nem/nail_care_and_timing_of_re_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ml9ltd</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Which shape suits me?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml9ltd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ml9g0z</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>What would be the best course of action fixing my mom's nails?</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml9g0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ml9c45</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Fluorescent nail polish. Yey or nay?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml9c45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ml8zdq</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Purple Cat Eye 💜</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml8zdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ml8gmp</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>End of summer mood</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ml8gmp/end_of_summer_mood/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ml8exb</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>So I decide to try shaping my own nails an wanted to know what you guys thought?</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml8exb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1mkvtwh</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>How do I make them healthy/pretty</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkvtwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ml4ohz</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml4ohz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ml78yi</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Help with rubber gel. Again.</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml78yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ml6tib</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Ouija set for witchy faire!</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml6tib</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1ml6n0c</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Honoring British railway semaphore signals</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml6n0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1ml5wed</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Octopus nails</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9pythttftuhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1ml61bu</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>4th use from these press ons!</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc690fifuuhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1ml5zyt</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Late to the game,but first time using gel polish!</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml5zyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1ml5zbc</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Should I book a builder gel appointment for my nails?</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml5zbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1ml5wdg</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>2 hours well spent 🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml5wdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1ml5pi5</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Not sure about the color</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55hykxa3suhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1ml5l6i</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Fun Summer Neon✨💕</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gv1v169ruhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1ml5cdr</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>My first attempt at gel.:)</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vpux9l8kpuhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1ml4xfv</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>My nails vs the inspo from @styledigits on Pinterest 🥲🥲</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml4xfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1mkqd9y</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Help me pick a shade!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkqd9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1mkvhcz</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Please help me</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkvhcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1ml3k51</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>What gel is this? (Instagram: Insomnianaails)</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3mhsd77duhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1ml2nfw</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Low harm options on strong natural nails?</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0qha9207uhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1ml3bbg</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>i got these done 6 days ago, does this look like a normal amount of growth?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml3bbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1ml3zup</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Which service should I select when scheduling?</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ml3zup/which_service_should_i_select_when_scheduling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ml2ofj</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Too basic?</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pp8zsjlx6uhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1ml260f</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>She slayed 💎</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxb7ftmq3uhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1ml1p9v</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Stacked ring nails</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kl95ir4l0uhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ml0ou4</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Where (else) did I go wrong with my gel application?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpe92juttthf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1ml0t50</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>cats eye</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml0t50</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1mkzhrb</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Purple and pink 😍</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkzhrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1mkzfyr</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>What shape should I go for? My stilettos have been annoying me a little. Any particular shape that fits my hands?</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkzfyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1mkynz5</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Loving this color</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkynz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1mkyfbc</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>help! what should i get (im clueless)</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkyfbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1mkte2b</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Looking for advice!!</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkte2b/looking_for_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1mksq5g</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>This is what happens when u gossip with ur nail tech 🌸</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mksq5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1mkshpk</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Was a nail biter - how to fix cuticles now I’ve grown out my nails</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkshpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1mkxwxd</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>advice for begginer</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkxwxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1mkx34m</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>I made the strawberry nails into a set!</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkx34m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1mkx329</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Which of these styles would you choose for your next manicure? 💅✨”</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkx329</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1mkwrqt</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Wedding Guest nails</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8oscxoj93thf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1mkwpqx</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Forever a chrome girlie 🤍</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gz7xwpcu2thf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1mkwj6g</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Is there a way I can get my nails done again?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkwj6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1mkvnjc</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Nails at home for the first time</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkvnjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1mkv52u</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>54 straight male. My personality reflects my nails 💅.</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkv52u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1mkushh</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Gingham ombre nails</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkushh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1mkuipo</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>I’m loving them</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkuipo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1mkuc2f</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>I’m now nail obsessed</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkuc2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1mktk5c</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Slowly getting used to my long stilettos 💜</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pm6kh4dyeshf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1mkt93x</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>i just want summer to be overrrr</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkt93x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1mksoug</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Black tip French</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mksoug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1mksn93</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>New chrome set</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mksn93</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1mksb0y</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Color-changing Nails for Ghost</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5on4wjhf3shf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1mkrrqi</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Why are people afraid of black polish?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkrrqi/why_are_people_afraid_of_black_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1mkrq86</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>What would you call this style?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qg87italxrhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1mkrkca</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Can’t get over how cute these turned out 😻</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkrkca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1mkr8dq</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Is it flattering for my skin tone?</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3f66aerasrhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1mkqfkd</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkqfkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1mkqdzq</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Staying off extensions to grow my natural nails and keep them healthy since my nails break ALOT. Got overlays with a neutral gel polish. Mom thinks I wasted my money and should’ve opted for a darker shade of polish. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hwrw6ztlirhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1mkpn4z</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>UV light exposure / advice</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mkpn4z/uv_light_exposure_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1mljymu</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>I was never an orange gal...</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mljymu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1mliqzw</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Difficult polishes lead to oily fingers</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/187qqi67wxhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1mlifoe</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>New storage and the mani that survived assembly</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlifoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1mlgn3c</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Neon summer</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlgn3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1mlfy7i</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Milky taupe base with strong reddish pink shimmer?</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlfy7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1mlfn7i</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Weekly press on nails question</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mlfn7i/weekly_press_on_nails_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1mlfmj9</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>I’m just a ghourl</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/929pf3a90xhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1mlfk4w</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>I do love an offputting polish name 💚</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m15ez0zkzwhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1mleysm</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>some more Blackheart Beauty!</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mleysm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1mlelj6</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>BKL All the Rage Collection &amp; Donations ?</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mlelj6/bkl_all_the_rage_collection_donations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1mle1pn</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Vanessa Molina Ocean Glint</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ohltm4hwlwhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1mldu3y</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Lime green polishes similar to Essie This or That?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mldu3y/lime_green_polishes_similar_to_essie_this_or_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1mlds6g</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Ya'll please help with polish removal! 🙏</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mlds6g/yall_please_help_with_polish_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1mld5wq</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Easy Yellow French Mani</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5padjc18ewhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1mlcojr</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>I love cirque but $14.50 for a LE jelly? Just 🙅‍♂️</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlcojr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1mlceeh</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Dupes for Lumens Aurora Beam</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mlceeh/dupes_for_lumens_aurora_beam/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1mlc7pi</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>This combo is so fun!</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlc7pi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1mlc6ky</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>This was pretty without flash, but with flash it's incredible</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wobmzyor5whf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1mlc20r</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>ILNP - Dark Matter 🚀</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bk4wqtro4whf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1mlbrs7</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Camping with Holo Taco new release</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gs1j5ps52whf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1mlbdqv</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Tiny Bubbles when nail polish dries</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl0a1yyzyvhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1mlavvt</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Opinions on polishes</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlavvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1mlavi3</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>BKL freebies - how do they work?</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mlavi3/bkl_freebies_how_do_they_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1mlahlr</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Tried to copy aculed, got bikini instead 😂</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlahlr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1mlafw1</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer Restock, including Riding Sleeping Bag… and F*ck This Sh*t</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlafw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1mla6xx</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Finally, my first Lurid order!</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mla6xx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1mla6s6</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Simultaneously doing velvet, unmagnetized, and cateye swatches</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mla6s6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1mla0cs</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>What’re yall’s brush setups like? 😭😭 (I need help figuring out mine)</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mla0cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1ml9sxa</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Low Tech Glass Bead + Stamping</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8419ey8vlvhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1ml9qj4</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Feeling old school doing a bar magnet 🫣 Deep Space you will always be that girl 💫</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml9qj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1ml9q3u</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>ILNP Magnetic Lacquer</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7l3k2srlvhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1ml9lwc</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Can you magnetize for *too* long?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ml9lwc/can_you_magnetize_for_too_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1ml9caa</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Names Cheetah, Chester cheetah</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml9caa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1ml9ahd</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>PI Colors - Chelonian in the Stars.000</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20bwzi0eivhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1ml978y</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Orb magnet design</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml978y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1ml8i4k</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Glass bead effect using magnetic stirrer - BKL Only One Bed</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6mo6vmv9cvhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1ml8ffn</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>6 feet under the stars ✨</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8xaczgsbvhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1ml8agw</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Glass bead with Kathleen &amp; Co “Molten Sky”</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rzxt0rnravhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1ml82nh</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Atomic Polish - Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml82nh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1ml7ls7</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>ILNP Vaporwave after a few days wear</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml7ls7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1ml7b8x</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>gel allergy question</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ml7b8x/gel_allergy_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1ml7aya</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Just some solar fun now that the sun is out in SF (technically not an ad but it’s our polish hence the tag)</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml7aya</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1ml6qup</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>I can’t open this bottle?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/groiuodjzuhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1ml6nga</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Dupes for Birefringence or Cygnus Loop?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ml6nga/dupes_for_birefringence_or_cygnus_loop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1ml61ai</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Glass bead the simple way…</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8p00xblcuuhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1ml61cq</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Had to put polish back on as soon as I felt up to it (anesthesia, boo)</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml61cq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1ml5v67</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Blessed With a Curse</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml5v67</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1ml5v0o</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Need an Orly Nail Defense alternative</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ml5v0o/need_an_orly_nail_defense_alternative/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1ml5rd1</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Mooncat - Mutiny vs. Forbidden Fruit Comparison Request</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>/r/mooncatpolish/comments/1mkhq50/mutiny_vs_forbidden_fruit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1ml5r6k</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Something summery 😌🫧</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml5r6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1ml5fvs</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>I owe this polish an apology (an apolishgy?)</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml5fvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1ml5bgb</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Local Group?</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgt5jd5epuhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1ml55nc</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>So many people said this didn't live up to the hype I was not expecting much.... but excuse me WHAT???</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xwc091jbnuhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1ml52du</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>70% off polish - Rite Aide Closing Sale</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxq0w64mnuhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1ml4zs0</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>The dream of a thousand cats</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml4zs0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1ml4ws0</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Nail Health Help! Peeling, Onycholysis?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml4ws0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1ml4q83</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Eternal WOAH</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml4q83</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1ml4k2o</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>My favorite stamp to date! Porcelain vibes!</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml4k2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1ml4jud</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>My favorite stamp to date! Porcelain vibes!</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml4jud</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1ml3xqb</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Forces of Evil dupe attempt</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3il2unnrfuhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1ml3u0y</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Tip wear and uneven nails can't keep this mani down</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml3u0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1ml3fmq</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Psychic Unicorn 🦄</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wgtra1abcuhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1ml399t</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Skittle mani dump!</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml399t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1ml36ed</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>wake up, get up, get out there</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml36ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1ml2woj</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>absolutely cursed nail day</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml2woj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1ml2rb2</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>KB Shimmer Bucketlist</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/263lklhq7uhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1ml2cmu</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>First mani with stamping!</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml2cmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1ml22qv</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Holo Taco Reflective Taco on The Floor is Guava</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml22qv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1ml1z8l</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Styx and Elementalist</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wo8wryzg2uhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1ml1vcq</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>nail polish that peels off :(</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml1vcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1ml1szd</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>just found my new favourite polish!</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlalzx0a1uhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1ml1cdg</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>REPOSTING PER MOD REQUEST:  Not very creative, like me? Glass bead method tool (magnetic stirrer) you can just buy online!</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4i66jwxixthf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1ml1b9s</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Chamaeleon nails</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ml1b9s/chamaeleon_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1ml17xh</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>THAT b*tch</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml17xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1ml0vh4</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>tried something new!</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ulcgs9r0vthf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1ml0tzz</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Does anyone know what brand / color this is?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml0tzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1ml0hpd</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>My base coat doesn't contain PVB so why do my nails look like this?</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yx60v4sgsthf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1ml05ww</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>I think we all know who this cult classic is by now</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxkspuoaqthf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1ml02fb</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Oh nooo, help please in finding a dupe?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wm341bcmpthf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1mkz5nl</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>ILNP Pyro and Starrily Golden Starlight</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/euy1ih9ijthf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1mkz0ka</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>One of the cutest nail oils I've seen!</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkz0ka</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1mkysiw</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Cirque Verdigris Jelly v Zoya Frida?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkysiw/cirque_verdigris_jelly_v_zoya_frida/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1mkymml</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>I Might Just Die on This Hill... But Can We Talk About Something?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkymml/i_might_just_die_on_this_hill_but_can_we_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1mkyfku</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Can you refill Holo Taco refill cartridge?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkyfku/can_you_refill_holo_taco_refill_cartridge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1mkbsm4</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Learn Manicure In Salon? | Help!</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkbsm4/learn_manicure_in_salon_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1mkt6cl</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Tom and Jerry 🥰 my favourit couple 😆😁</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hgaqtlmgbshf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1mky5ht</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Rainbow nails 🌈</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4txy4edscthf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1mky1kw</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Beaux Reves Lagoon 💙</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mky1kw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1mkxitu</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Advice on shaping natural nails? feat. Nails Inc - Sofia</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkxitu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1mkxdmq</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Love nail polish but have terrible skin picking issues...</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh6ey21i7thf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1mkx7rf</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Swatch request: Chicago Fire vs You of Unshakable Conviction</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkx7rf/swatch_request_chicago_fire_vs_you_of_unshakable/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1mkx62c</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>ILNP Blue Lagoon is so stunning</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g65hp2916thf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1mkwrmo</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>My entire camera roll rn...</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkwrmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1mkwf4j</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Favorite Oxblood/Wine Red?</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkwf4j/favorite_oxbloodwine_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1mkw51m</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Memento mori</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0gb0l3syshf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1mkvv8s</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>LynB Sale Code?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkvv8s/lynb_sale_code/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1mkvjx5</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Welp 👀</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkvjx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1mkvje4</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Stripey</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/loaf7q0iushf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1mkvea1</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Selkie Atomic</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkvea1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1mkv7bx</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Looking for the bloodiest shimmer</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mkv7bx/looking_for_the_bloodiest_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1mlk0xl</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>first post! sharing nail arts from the past year and a half</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlk0xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1mlj1k0</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>I might just make the full set</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnd44izhzxhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1mli4er</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Stained glass nails</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mli4er</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1mlgkva</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Bioshock nail art</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q3q6gtyl8xhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1mlg0ph</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>cherries gone high fashion 🖤🍒🤍</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwycbzwv3xhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1mlfjwl</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Chocolate ice cream nails I made today!</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlfjwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1mlfg68</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Found The Cursed nail my sister warned me not to wear ....now it wont come off</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlfg68</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1mle4hs</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Cat Paw nails- first try!</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mle4hs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1ml9zy0</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>I feel like whenever I try something outside of landscapes it fails. Idk how you all do it...</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml9zy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1ml9zx8</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Thoughts on dollar tree nail supplies</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ml9zx8/thoughts_on_dollar_tree_nail_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1ml8p8b</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Happy Cat Day! 🐾 ❤️ 🐈</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml8p8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1ml77jz</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Princess energy :')</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ml77jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1ml6lgc</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Recent practice</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ix1k6gcgyuhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1ml1qox</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Ring stacked set✨</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cu288h5u0uhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1mkzgsp</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Just a girl and her Fresca 🍊✨</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkzgsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1mkwhsq</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Purple Paradise 😍💜</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkwhsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1mkxbye</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Put the strawberry nails in a set!</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkxbye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1mkwz5l</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>My first time doing 3D sculpted nails, I went for a sea animal theme</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkwz5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1mkwt7d</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Enchanted fairy forest bug nails</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkwt7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1mkwg50</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>some nails with good vibes!</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikmbf19y0thf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1mkuq1l</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Barbie inspired nails 💅🏼 I loooooove them!! 💕</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yy7wrpidoshf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1mkrln8</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Show girl press on nails I made</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mkrln8</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Aug 10 08:11:45 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_10.xlsx
+++ b/data/collected_data/2025_08_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1310"/>
+  <dimension ref="A1:C1512"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22703,6 +22703,3440 @@
         </is>
       </c>
     </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1mmcvfs</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>First time french tips</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mmcvfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1mmcsz6</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Haven't had french in sooo looong</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mmcsz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1mmcpts</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Old ones might delete later</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjp2ttqbe5if1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1mmc6mi</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mmc6mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1mmawqg</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>these nails are so pretty up-close but does it look dirty from afar?</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mmawqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1mmbqrc</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Rubber ducky nails</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mmbqrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1mmbpxa</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Silent hill nailss</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mmbpxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1mmbmxa</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Cat eye chocolate mint 🍫🍃</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbucm42025if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1mmbj4y</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Sunshine on the tips, flowers in full bloom</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3hl6p4r05if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1mmauzx</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>life is strange themed nails!!</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mmauzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1mm8kf6</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Gold chrome &amp; pink flowers (swipe for my chatgpt prompt to get my inspo!) 🌷</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm8kf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1mm9c7u</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Looking for a new product in US</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm9c7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1mm9ogj</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Husband helped with what to put on my nails :)</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm9ogj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1mma7ot</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Basic but cute.</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/igeyxt2dm4if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1mm9zef</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>How do we feel about the pastel yellow chrome look?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm9zef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1mm9k6q</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Nude shades never go out of style</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm9k6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1mm8t74</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Glow in the dark lava lamp nails</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0i0fc6ej84if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1mm8lcx</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>How can I become a nail tech?</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mm8lcx/how_can_i_become_a_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1mm8j1j</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>These shellacs are a month old. At what point do I do something? I’m starting to think they’re invincible 😅</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/un1kefbr54if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1mm8dor</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>She got her set and she’s loving it ✨</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cvu2cbx844if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1mm7yjc</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Did my own nails. ❤️</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yl2grt2b04if1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1mm794g</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Acrylic removal results</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4va09jvt3if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1mm7bms</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>How do I take care of dip powder nails?</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mm7bms/how_do_i_take_care_of_dip_powder_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1mm72br</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Galaxy Dust Nails</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm72br</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1mm739c</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>First time getting nails done at a salon. Please help</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm739c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1mm7taq</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>First Mani in 6 Years!</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm7taq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1mm74jf</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Ducky ducky</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm74jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1mm6lb8</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Love my new nail tech and absolutely in love with these</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm6lb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1mm5k32</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>What primer was this?</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mm5k32/what_primer_was_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1mm6bj9</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Advice please 💚</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylnz0dmhl3if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1mm5w8v</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Gel Manicure With Flower Design</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydbwbuxmh3if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1mm5p9y</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>New nails 🌸</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39x5m2rxf3if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1mm4rm6</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Opinions needed</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nf4i5d4k73if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1mm4gar</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Anyone else paint their nails while fishing?</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqn6zw0k43if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1mm4zzv</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Got my nails done 3wks ago</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6f5yu4m93if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1mm4rn2</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Practicing some different techniques 🧜🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tbb0382k73if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1mm4fmi</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>First Time Gel X</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm4fmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1mm2xe7</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Long-Lasting, Non-Damaging Adhesive for Reusable Press-On Nails??</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5k5jkaapr2if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1mm41fz</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucbu7mp613if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1mm3evg</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>New Russian mani🩵</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hpuyhiqv2if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1mm336r</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Got these done today yayyy</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yioh8mo1t2if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1mm2wro</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Can you tell I'm yearning for fall?</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm2wro</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1mm2vyq</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Love this pink combo 💓💓💓</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7p58ml3dr2if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1mm1e6z</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>How do I know if I have fungus under acrylics??</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mm1e6z/how_do_i_know_if_i_have_fungus_under_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1mm2f5d</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Second attempt at gel-x using the luminary system</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm2f5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1mm28kl</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Is there a nail shape that’s in between oval and almond?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm28kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1mm28ir</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>first spooky set of the season👻🍂</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm28ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1mm19ml</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Daisy nails</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obphmk5ae2if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1mm0zlv</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Broken nail help?</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dgpjvw2c2if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1mm0swj</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>So dreamy😍😍</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s3rqbbila2if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1mm0khb</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Why do they do this?</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm0khb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1mm06ie</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>After months of growth, this happened today.</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6n6qs7x52if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1mm058t</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>My natural nail growth</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0qkdoro52if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1mm04no</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Nail chipped under shellac</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qj7w8zek52if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1mlzq20</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Do u like my nails?</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qo02q50h22if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1mlzm6u</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Second time getting nails done professionally. I rather like the chrome powder thing</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqonfhxm12if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1mly3s1</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Do salons record how much you tip?</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mly3s1/do_salons_record_how_much_you_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1mly22q</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>What's this darker red/purple above my lunula? And are these Muehrcke's lines (other pics)</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mly22q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1mlnhy9</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Pitting at the base of nail after removing press ons</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlnhy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1mltr6e</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>acrylic before biab?</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mltr6e/acrylic_before_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1mlts1l</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlts1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1mlxz6s</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Polygel/Hybrid gel Lotus Nails</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f25hyc8p1if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1mlw7au</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Nail health/aesthetic??</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5v7yim0c1if1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1mlxu0u</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Barbie nails 🩷</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyip7cf5o1if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1mlxovn</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Koi fish set</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7d75xzu1n1if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1mlws9z</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Might have just made my fav set ever 💜🦋</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlws9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1mlwmfk</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>"I not going to get sucked into the gel rabbit hole" is what I tell myself.. but they look so good lol</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sffxwjr6f1if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1mlwhnm</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Is it too early for Halloween 👻</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlwhnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1mlw4qh</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>in love with her</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6lnul3bgb1if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1mlvsiu</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>new set, who dis</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlvsiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1mlvqq6</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>New set that I made ❤️🖤🤍</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gncpvsdo81if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1mlvqkh</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Traffic Cone Neon Orange Nails</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlvqkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1mlvhuj</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlvhuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1mlvfwd</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Nails I did on my boyfriend</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlvfwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1mlv29k</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Nail techs: Solve a dispute for me… is this unacceptable to get a pedicure? (NSFW cuz not pretty painted nails lol)</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtucaihq31if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1mlto67</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Nails for the bad bunny residency in Puerto Rico.</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2gwuy6yet0if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1mltdje</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Ice cream you scream, we all scream for ice cream!</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vc4bkj8r0if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1mlstyc</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>What product would be best for really thin and weak nails?</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjg1cljbn0if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1mlslsf</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Second set of at home gel X</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/untogienl0if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1mls7wg</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Cat eye on natural nails 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mls7wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1mls77r</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Is it pretty?</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23h7feioi0if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1mlryka</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>When to get a refill?</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dk33p5aug0if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1mlrwh1</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>I had to share my sponge bob nails with y'all</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i7m9tf6eg0if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1mlrmiz</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Goth nails</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlrmiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1mlr8qr</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Which of these is healthier for my nails? (Or does it not make a difference)</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlr8qr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1mlqzyq</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Hiii, how i get rid of the Dust on the border of my chromes</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3q42kfk90if1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1mlqp5p</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>My nail journey since May</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlqp5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1mlq6nk</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Are top and base coat damaging to your nails?</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mlq6nk/are_top_and_base_coat_damaging_to_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1mlq385</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Getting better! Open to constructive criticism</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlq385</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1mlpofc</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Got my nails done at a salon for the first time</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9ryx8vzyzhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1mlou8v</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>New stick ons</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlou8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1mloobg</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Tried to have natural looking nails for a while but I love glitter and glitter loves me</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qfs5hy6hqzhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1mlocgt</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>What type of gel is this?</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lyqtry6nzhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1mlo0me</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Are my expectations too high</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlo0me</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1mlny19</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Getting ready for fall(still months away)</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlny19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1mlneiw</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Wrong pink</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlneiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1mln8ut</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>What's a good toe nail color/design that goes with any manicure?</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mln8ut/whats_a_good_toe_nail_colordesign_that_goes_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1mln2xz</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Starting nails?</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mln2xz/starting_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1mln0rt</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Decided to try a bright red, still not sure if I like it</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ni4kbvex3zhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1mlmxiv</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Grey kind of day</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhmed5xa9zhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1mmbasy</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Emily de Molly shimmers, chefs kiss</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mmbasy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1mmb7t2</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Wearing Playing with Sapphire while playing with sapphire from Sapphire</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mmb7t2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1mmb061</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Advice on what to buy and general nail advice?</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mmb061</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1mmakhh</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Subtle pink frenchie!</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oizc1555q4if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1mmaalx</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>My first jelly sandwich matches the wildflowers :)</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bk6f9bu9m4if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1mm94t9</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>New shade</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/weucd89ib4if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1mm8wxc</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Another Abstract Mani 🩵</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm8wxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1mm8i5w</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Help, what is this "dead" spot on my index finger?</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm8i5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1mm89sf</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>10 months of not biting my nails, I've made amazing progress.</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm88w0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1mm7w43</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>my fishies bring all the kitties to the yard 🐠🐟</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xzqt658oz3if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1mm7klk</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>OPI Summer For Shore</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8tkrh0sw3if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1mm79cz</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Finally happy with my manicures - ILNP Eclipse</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7q0x5er3q3if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1mm74nd</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>My fiancé did my nails 💅 by</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm74nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1mm6pra</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Oil spill</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d4b4awgyo3if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1mm6nm8</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>First dark sparkling polish- obsessed!</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/akpbhmjfo3if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1mm6665</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Am I still allowed if I didnt use a magnet? 🫣</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm6665</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1mm5sea</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Legos acquired! Glass bead unlocked! I love this community.</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1jipp8oag3if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1mm5r1h</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>Juicy jam nails</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm5r1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1mm5cl6</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Day Tripper + Magnetic Taco + Sparkling Blush = 💕</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rnxv7pmpc3if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1mm58ps</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>When freshly sharpened talons meet a super shifty  polish 🐉🔮✨</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm58ps</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1mm55rq</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Flakies are hard y’all</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm55rq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1mm50fp</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Magnetic stirrer for the WHOA</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fqy0rngj93if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1mm4x2a</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Finally got The Sea Haunt the other day</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm4x2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1mm4l4y</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Facebook Marketplace score for $40!</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm4l4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1mm4ik6</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>So excited for this Sassy Sauce combo</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iptfa9sa53if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1mm4b1p</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Are these too similar?</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm4b1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1mm48x7</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Petals and Mutagen by ILNP</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm48cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1mm43jf</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>First attempt at skittle mani</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm43jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1mm3zbb</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Seawinkle - Dreamland Lacquer 💜</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm3zbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1mm3r0o</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Day 1 vs day 13 vs day 16 of my dazzle dry mani</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm3r0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1mm3nlf</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Another Estate Haul</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxa4y65ux2if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1mm3jqu</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>starting from absolute ground 0—what are some of your go-to lacquers?</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mm3jqu/starting_from_absolute_ground_0what_are_some_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1mm2nd2</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Tortoiseshell 🥰</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm2nd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1mm2fn5</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Matchy Matchy!</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vx5ynk0on2if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1mm27ig</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>This subreddit made me try lacquer again</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm27ig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1mm1nrp</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Nail Clippers</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mm1nrp/nail_clippers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1mm1jvu</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Wave FC</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73t3nwzcg2if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1mm195z</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Lint free cotton pads?</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mm195z/lint_free_cotton_pads/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1mm17e7</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Does anyone have a comparison of Holo Taco’s Ivory Tower and ILNP’s Soulmate?</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mm17e7/does_anyone_have_a_comparison_of_holo_tacos_ivory/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1mm0e40</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>🔥 Kathleen &amp; Co Follow Your Dreams ♥️🧡</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm0e40</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1mlztdh</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>So gorgeous in the sun</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b74y00f632if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1mlzeq3</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>I just jumped right in!</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlzeq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1mlz41x</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>We have neon coral with blue shimmer at home</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlz41x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1mlyngs</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>How to fix nail lifting/hang nail</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbbsn44du1if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1mlyhck</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>Cirque Paradiso (in space)</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1nojqy2t1if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1mly3pl</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>question: can i use le mini macaron metal powder over regular polish?</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gli0h5z6q1if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1mlxs0g</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>How bad of an idea would it be to use cheap-ish gel polishes (Aliexpress, Shein, etc) on top of safe and regulated ones?</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mlxs0g/how_bad_of_an_idea_would_it_be_to_use_cheapish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1mlxmhq</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Any jelly tips/ideas!</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mlxmhq/any_jelly_tipsideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1mlxl55</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Can someone show the difference between velvet and glass bead?</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mlxl55/can_someone_show_the_difference_between_velvet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1mlxdly</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>I love a spooky summer.</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p72ls3pjk1if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1mlx72d</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Full STEM ahead!!!</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wciujathj1if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1mlx4f0</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Indies with cyan(ish) shimmer</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlx4f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1mlwfd9</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>Vacation mani - Alaska</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlwfd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1mlvqwu</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Showing some love to a local brand</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlvqwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1mltsho</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>How often do yall change your polish?</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mltsho/how_often_do_yall_change_your_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1mltl14</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Lynb collection availability during sale?</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mltl14/lynb_collection_availability_during_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1mltjp1</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Memphis 🔵</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mltjp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1mlth4z</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>It's my birthday!</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/feq4h1rzr0if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1mltfs9</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>ILNP Hypnosis</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7j7evp9qr0if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1mlt5oc</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>By the light of the moon</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k5yjg2zmp0if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1mlg89h</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Bioshock nail art</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s5likate5xhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1mlspvd</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>UPDATE: Magnetic Stirrer &amp; the Glass Bead Effect</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xy4t5uzcm0if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1mlso65</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>Cracked Polish Base Coats and QDTC</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mlso65/cracked_polish_base_coats_and_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1mls2bq</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>My first attempt at glitter ombre</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mls2bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1mls0xy</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>Some Saturday Swatching</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0uxlmr1ch0if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1mlrrro</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Help me build my first ILNP order!</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlrrro</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1mlr9k1</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>I further destroyed this mani about 5 minutes after this picture was taken, but it was gorgeous while it lasted 🤩</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ls0109hlb0if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1mlr6x8</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>Peridot-ish?</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlr6x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1mlqqmp</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Thumb jail</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlqqmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1mlpbes</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Similar intensity/finish neons to Sour Apple Rings? Orange, red, purple, ESPECIALLY blue!</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ah2wx88xvzhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1mlp396</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Anyone remember Art Stuff??</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3j9sye1uzhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1mlp1ih</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Polish August HHC exclusive- Swatch in motion</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w1ihf8smtzhf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1mloz1p</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Pretty Purple</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mloz1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1mlniga</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>Green for August!</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrkd5bkefzhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1mlmpof</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>Are the CND products in Amazon UK legit?</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mlmpof/are_the_cnd_products_in_amazon_uk_legit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1mlmonb</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Believe the hype!</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1ydblij6zhf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1mlll7t</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Does anyone know what shade this vintage Sinful nail polish is?</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfjrqzrwryhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1mlkt25</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Smudge free top coat recommendations in Europe ?</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mlkt25/smudge_free_top_coat_recommendations_in_europe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1mlkhrj</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>How to get glass bead with wand?</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sifcj4jegyhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1mm9rv4</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>Felt proud enough to share :)</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm9rv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1mm8fmw</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Work in progress 💚</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm8fmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1mm6qlr</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>Kashy taila nails.</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/elssl5p5p3if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1mm6ccc</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>ordering nails from you guys</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mm6ccc/ordering_nails_from_you_guys/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1mm64ho</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>Gel Manicure With Flower Design</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mm64ho/gel_manicure_with_flower_design/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1mm62xu</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>I paid $160 for detailed art but acrylics was 20% off australia chatswood</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mm62xu/i_paid_160_for_detailed_art_but_acrylics_was_20/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1mm4rzo</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>Cat nails 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm4rzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1mm2n9j</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>My first builder gel</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm2n9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1mm1ipg</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>How to achieve something like this?</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwu7s93cg2if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1mm16mv</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>Glue help</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mm16mv/glue_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>1mm0zje</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>little roses are hard, pls tips for painting roses</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/488sdwe2c2if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr">
+        <is>
+          <t>1mm086x</t>
+        </is>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>How to stop chipping?</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mm086x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr">
+        <is>
+          <t>1mlxo4y</t>
+        </is>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>Dripping gold, staring bold 💛👁️</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfu1rj1xm1if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>1mlx4qv</t>
+        </is>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>should I make the full set ...🫣</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlx4qv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr">
+        <is>
+          <t>1mlwrhr</t>
+        </is>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>BEETLEJUICE, BEETLEJUICE, BEETLEJUICE</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlwrhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>1mlwet2</t>
+        </is>
+      </c>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>My client today asked for this design, perfect for summer</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/842m2rakd1if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>1mlvwvr</t>
+        </is>
+      </c>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>First time with 3D gel— literally any tips welcome lol</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlvwvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>1mlvl7d</t>
+        </is>
+      </c>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>Is it too early for Halloween 👻</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlvl7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>1mlqyts</t>
+        </is>
+      </c>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>Pink vibey aura nails just for fun 🩷❤️🩷🥰</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kr0144db90if1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>1mlpqfl</t>
+        </is>
+      </c>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>added some glitter</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlpqfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>1mlphhb</t>
+        </is>
+      </c>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>Is super glue safe for acrylics?</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2nfnftdxzhf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>1mlnrqx</t>
+        </is>
+      </c>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>Kpop demon hunters set</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlnrqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>1mlkn5p</t>
+        </is>
+      </c>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>The dream of a thousand cats</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mlkn5p</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>